<commit_message>
getting close, and done for the day
</commit_message>
<xml_diff>
--- a/Berthierine calculator.xlsx
+++ b/Berthierine calculator.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cromp\Desktop\clay_thermo\clay-thermodynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="12530" windowHeight="6840"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12525" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1429,7 +1424,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -1541,7 +1536,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1591,7 +1586,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1641,7 +1636,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1719,7 +1714,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1752,26 +1747,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1804,23 +1782,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2000,18 +1961,18 @@
   <dimension ref="A3:AE45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="13.6328125" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="10:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="10:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="W3" t="s">
         <v>41</v>
       </c>
@@ -2034,7 +1995,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V4" t="s">
         <v>42</v>
       </c>
@@ -2066,7 +2027,7 @@
         <v>22.97</v>
       </c>
     </row>
-    <row r="5" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V5" t="s">
         <v>43</v>
       </c>
@@ -2098,7 +2059,7 @@
         <v>27.26</v>
       </c>
     </row>
-    <row r="6" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V6" t="s">
         <v>44</v>
       </c>
@@ -2130,7 +2091,7 @@
         <v>32.47</v>
       </c>
     </row>
-    <row r="7" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V7" t="s">
         <v>45</v>
       </c>
@@ -2162,7 +2123,7 @@
         <v>24.98</v>
       </c>
     </row>
-    <row r="8" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V8" t="s">
         <v>46</v>
       </c>
@@ -2194,7 +2155,7 @@
         <v>25.91</v>
       </c>
     </row>
-    <row r="9" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V9" t="s">
         <v>47</v>
       </c>
@@ -2226,7 +2187,7 @@
         <v>21.61</v>
       </c>
     </row>
-    <row r="10" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V10" t="s">
         <v>48</v>
       </c>
@@ -2258,7 +2219,7 @@
         <v>34.96</v>
       </c>
     </row>
-    <row r="11" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V11" t="s">
         <v>49</v>
       </c>
@@ -2290,7 +2251,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="12" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="V12" t="s">
         <v>50</v>
       </c>
@@ -2322,7 +2283,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="13" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="K13" t="s">
         <v>28</v>
       </c>
@@ -2357,7 +2318,7 @@
         <v>4.57</v>
       </c>
     </row>
-    <row r="14" spans="10:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="10:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="K14" t="s">
         <v>21</v>
       </c>
@@ -2404,7 +2365,7 @@
         <v>14.23</v>
       </c>
     </row>
-    <row r="15" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="J15" t="s">
         <v>19</v>
       </c>
@@ -2454,7 +2415,7 @@
         <v>46.72</v>
       </c>
     </row>
-    <row r="16" spans="10:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="10:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="J16" t="s">
         <v>22</v>
       </c>
@@ -2504,7 +2465,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>23</v>
       </c>
@@ -2530,7 +2491,7 @@
         <v>-287.2</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" ht="14.45" x14ac:dyDescent="0.35">
       <c r="J18" t="s">
         <v>24</v>
       </c>
@@ -2541,7 +2502,7 @@
         <v>-290.79000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2557,7 +2518,7 @@
         <v>-0.85699999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2568,7 +2529,7 @@
         <v>-0.57899999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +2540,7 @@
         <v>-0.108</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -2611,7 +2572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>9</v>
       </c>
@@ -2622,7 +2583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -2663,7 +2624,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -2707,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -2724,7 +2685,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>89</v>
       </c>
@@ -2732,7 +2693,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -2809,7 +2770,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>51</v>
       </c>
@@ -2906,7 +2867,7 @@
         <v>1.3840896296296294</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>52</v>
       </c>
@@ -2999,7 +2960,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="33" spans="2:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>53</v>
       </c>
@@ -3092,7 +3053,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="34" spans="2:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>54</v>
       </c>
@@ -3108,7 +3069,7 @@
         <v>9.0009999999999994</v>
       </c>
     </row>
-    <row r="35" spans="2:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>54</v>
       </c>
@@ -3121,7 +3082,7 @@
         <v>-204.03000000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>55</v>
       </c>
@@ -3158,7 +3119,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="2:31" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:31" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>56</v>
       </c>
@@ -3203,7 +3164,7 @@
         <v>-3513.969747024456</v>
       </c>
     </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C38">
         <f>SUM(C31:C37)</f>
         <v>-1812.9016256250002</v>
@@ -3244,7 +3205,7 @@
         <v>-839.49776554647985</v>
       </c>
     </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G39">
         <f>1*W12*0.5</f>
         <v>-146.375</v>
@@ -3257,7 +3218,7 @@
         <v>1276.7017499999999</v>
       </c>
     </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G40">
         <f>3*W12*0.5</f>
         <v>-439.125</v>
@@ -3270,7 +3231,7 @@
         <v>344.94957784999997</v>
       </c>
     </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G41">
         <f>SUM(G32:G40)+J31</f>
         <v>-3824.6024273617058</v>
@@ -3294,7 +3255,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G42">
         <f>2*G41</f>
         <v>-7649.2048547234117</v>
@@ -3321,7 +3282,7 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
         <v>114</v>
       </c>
@@ -3344,7 +3305,7 @@
         <v>2.0158800000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C44">
         <f>0.667*0.25/2</f>
         <v>8.3375000000000005E-2</v>
@@ -3353,7 +3314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
       <c r="C45">
         <f>C44*3</f>
         <v>0.25012500000000004</v>
@@ -3376,7 +3337,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3388,7 +3349,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>